<commit_message>
finish working celebration list
</commit_message>
<xml_diff>
--- a/document/基本設計書/お祝い.xlsx
+++ b/document/基本設計書/お祝い.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\azusato\document\基本設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C278498C-BF98-4C79-96C7-8B3810C10CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A26420-46F0-470C-9DFB-FFD12456ED2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2910" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="110">
   <si>
     <t>ページ</t>
     <phoneticPr fontId="1"/>
@@ -765,6 +765,24 @@
     <rPh sb="7" eb="9">
       <t>ショリ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>read_count</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>読んだ数</t>
+    <rPh sb="0" eb="1">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>スウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>number</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -796,12 +814,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -816,7 +840,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -826,6 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4090,8 +4115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4180,18 +4205,18 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B20" t="s">
+      <c r="B20" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
@@ -4307,10 +4332,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97434556-6B23-4BF1-9CB6-03B00EDF4972}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4493,78 +4518,75 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="D22" t="s">
         <v>26</v>
@@ -4572,13 +4594,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
         <v>26</v>
@@ -4586,41 +4608,41 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
@@ -4628,182 +4650,182 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>64</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>62</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" t="s">
-        <v>15</v>
-      </c>
-      <c r="C33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>14</v>
       </c>
       <c r="B34" t="s">
-        <v>76</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
         <v>22</v>
       </c>
+      <c r="D35" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.4">
+      <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A38" s="3" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A39" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="D39" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D42" t="s">
         <v>26</v>
@@ -4811,15 +4833,29 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>42</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>43</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>44</v>
       </c>
     </row>
@@ -4918,8 +4954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB63D199-DE6C-43DE-9E1E-C8D76622D48E}">
   <dimension ref="K34:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
finish celebration page html
</commit_message>
<xml_diff>
--- a/document/基本設計書/お祝い.xlsx
+++ b/document/基本設計書/お祝い.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\azusato\document\基本設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A26420-46F0-470C-9DFB-FFD12456ED2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC017001-535C-4272-95BA-E0A8C9597F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2910" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -3315,8 +3315,12 @@
           </a:br>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>クリックするとプロフィール変更可能</a:t>
+            <a:t>クリックするモーダルが出てとプロフィール変更可能</a:t>
           </a:r>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+          </a:br>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3841,6 +3845,318 @@
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>戻る</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rectangle 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD99CB5F-A3FD-41A8-B1A3-2B9EF2C90F6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6496050" y="2581275"/>
+          <a:ext cx="2324100" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83E575A6-F3BD-4575-9FFB-DC80A3D36544}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6524625" y="2647950"/>
+          <a:ext cx="2000250" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>プロフィール写真変更</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rectangle 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D3AD5D4-DDC6-47D8-A318-1E4CCF529028}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6562725" y="2990849"/>
+          <a:ext cx="2000250" cy="676276"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>プロフィール写真変更を行いますか？</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Rectangle 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0A58A1E-0BCC-45AC-A809-24D776AAAE1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7477125" y="3762375"/>
+          <a:ext cx="542925" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>変更</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rectangle 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07377AB2-E72A-402D-9EAE-684576C5BA1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8001000" y="3752850"/>
+          <a:ext cx="657225" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>いいえ</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4115,8 +4431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4210,14 +4526,16 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
+      <c r="B21" s="5" t="s">
         <v>53</v>
       </c>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>54</v>
       </c>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
@@ -4334,8 +4652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97434556-6B23-4BF1-9CB6-03B00EDF4972}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4869,7 +5187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAD6C30-5A6A-4F1A-A99D-6F71EF6C1A28}">
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -4954,7 +5272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB63D199-DE6C-43DE-9E1E-C8D76622D48E}">
   <dimension ref="K34:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -5041,8 +5359,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD9DB05-932A-4FAA-A0C5-773A5804E9B9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
modify & add documents
</commit_message>
<xml_diff>
--- a/document/基本設計書/お祝い.xlsx
+++ b/document/基本設計書/お祝い.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\azusato\document\基本設計書\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\azusato\document\基本設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC017001-535C-4272-95BA-E0A8C9597F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AB608F-DC56-441F-974D-6749C181012D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1830" yWindow="2865" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="116">
   <si>
     <t>ページ</t>
     <phoneticPr fontId="1"/>
@@ -198,22 +198,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>loginテーブルのFK</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>String(50)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>名前</t>
-    <rPh sb="0" eb="2">
-      <t>ナマエ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -412,10 +401,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>need_read</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>String array</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -427,19 +412,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>これを確認する必要がある人</t>
-    <rPh sb="3" eb="5">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ヒト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・お祝い+お祝い書き込みのneed_readの数を表示</t>
     <rPh sb="2" eb="3">
       <t>イワ</t>
@@ -521,14 +493,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>login</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ログイン</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -542,32 +506,6 @@
   </si>
   <si>
     <t>ユーザタイプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1:管理者
-2:非ログイン
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="游ゴシック"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3:KAKAOログイン
-4:Lineログイン</t>
-    </r>
-    <rPh sb="2" eb="5">
-      <t>カンリシャ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ヒ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -783,6 +721,81 @@
   </si>
   <si>
     <t>number</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>profile_image</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロフィール管理テーブル</t>
+    <rPh sb="6" eb="8">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>profile_image_no</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロフィール管理テーブルFK</t>
+    <rPh sb="6" eb="8">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FK</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1:管理者
+2:非ユーザ
+3:KAKAOユーザ
+4:Lineユーザ</t>
+    <rPh sb="2" eb="5">
+      <t>カンリシャ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ヒ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>userテーブルのFK</t>
+  </si>
+  <si>
+    <t>ユーザ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unread_user</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>まだ確認していない人</t>
+    <rPh sb="2" eb="4">
+      <t>カクニン</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ヒト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お祝い番号</t>
+    <rPh sb="3" eb="5">
+      <t>バンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ユーザID</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4431,8 +4444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4454,7 +4467,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -4469,35 +4482,35 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
@@ -4512,28 +4525,28 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B20" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B21" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B22" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C22" s="5"/>
     </row>
@@ -4544,70 +4557,70 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C26" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B29" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C30" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="C32" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B33" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C34" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.4">
       <c r="C36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4622,7 +4635,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4650,10 +4663,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97434556-6B23-4BF1-9CB6-03B00EDF4972}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4677,7 +4690,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -4715,16 +4728,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -4735,49 +4748,49 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -4785,143 +4798,143 @@
         <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>107</v>
-      </c>
-      <c r="B15" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" t="s">
-        <v>109</v>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
         <v>49</v>
       </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>20</v>
-      </c>
       <c r="D21" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
         <v>24</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
@@ -4929,182 +4942,185 @@
         <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
         <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>113</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>63</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="s">
         <v>15</v>
       </c>
-      <c r="B32" t="s">
-        <v>75</v>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="75" x14ac:dyDescent="0.4">
+      <c r="A36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A37" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A38" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>80</v>
+      <c r="B37" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A39" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>26</v>
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
@@ -5112,69 +5128,166 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
         <v>37</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D41" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>30</v>
+      </c>
+      <c r="B49" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>32</v>
+      </c>
+      <c r="B51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" t="s">
         <v>41</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D53" t="s">
         <v>42</v>
-      </c>
-      <c r="C44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -5198,37 +5311,37 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D10" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -5239,17 +5352,17 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D15" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
@@ -5257,7 +5370,7 @@
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.4">
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -5280,72 +5393,72 @@
   <sheetData>
     <row r="34" spans="11:13" x14ac:dyDescent="0.4">
       <c r="K34" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L35" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M36" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L37" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M38" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L39" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M40" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="11:13" x14ac:dyDescent="0.4">
       <c r="K42" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L43" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M44" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L45" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M46" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L47" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M48" s="2" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -5367,7 +5480,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push modified all codes
</commit_message>
<xml_diff>
--- a/document/基本設計書/お祝い.xlsx
+++ b/document/基本設計書/お祝い.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\azusato\document\基本設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AB608F-DC56-441F-974D-6749C181012D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AE594A-9D4E-4067-A696-2A0CEE4223FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1830" yWindow="2865" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="2400" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
-    <sheet name="データベース" sheetId="2" r:id="rId2"/>
-    <sheet name="テーブル" sheetId="3" r:id="rId3"/>
-    <sheet name="header" sheetId="6" r:id="rId4"/>
-    <sheet name="リストページ" sheetId="4" r:id="rId5"/>
-    <sheet name="作成・修正ページ" sheetId="7" r:id="rId6"/>
+    <sheet name="テーブルER図" sheetId="3" r:id="rId2"/>
+    <sheet name="class図" sheetId="8" r:id="rId3"/>
+    <sheet name="header(html)" sheetId="6" r:id="rId4"/>
+    <sheet name="リストページ(html)" sheetId="4" r:id="rId5"/>
+    <sheet name="作成・修正ページ(html)" sheetId="7" r:id="rId6"/>
+    <sheet name="リストページ" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,17 +42,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>ページ</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>データベース</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>・テーブル</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -81,275 +79,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>結婚のお祝いを記録しておきたい。できれば、書き込みと通知ができて1回だけのやり取りができればと思います。</t>
-    <rPh sb="0" eb="2">
-      <t>ケッコン</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>イワ</t>
-    </rPh>
-    <rPh sb="7" eb="9">
-      <t>キロク</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ツウチ</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>カイ</t>
-    </rPh>
-    <rPh sb="39" eb="40">
-      <t>ト</t>
-    </rPh>
-    <rPh sb="47" eb="48">
-      <t>オモ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>URL,ID,passwordは環境変数を利用</t>
-    <rPh sb="16" eb="20">
-      <t>カンキョウヘンスウ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>リヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>本番：Amazon-mysqlを利用(無料ですので)</t>
-    <rPh sb="0" eb="2">
-      <t>ホンバン</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ムリョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ローカル：ローカル-mysqlを利用</t>
-    <rPh sb="16" eb="18">
-      <t>リヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テーブル名</t>
-    <rPh sb="4" eb="5">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>celerbration</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>フィールド</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>no</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>物理名</t>
-    <rPh sb="0" eb="3">
-      <t>ブツリメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>論理名</t>
-    <rPh sb="0" eb="3">
-      <t>ロンリメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>備考</t>
-    <rPh sb="0" eb="2">
-      <t>ビコウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>番号</t>
-    <rPh sb="0" eb="2">
-      <t>バンゴウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PK,Autio_increment</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Number</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>String(50)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>String(10)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>not null</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイトル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>content</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>内容</t>
-    <rPh sb="0" eb="2">
-      <t>ナイヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>text</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>create_datetime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>作成日時</t>
-    <rPh sb="0" eb="2">
-      <t>サクセイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ニチジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>update_datetime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>create_user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>update_user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>作成者</t>
-    <rPh sb="0" eb="3">
-      <t>サクセイシャ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>更新日時</t>
-    <rPh sb="0" eb="2">
-      <t>コウシン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ニチジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>更新者</t>
-    <rPh sb="0" eb="3">
-      <t>コウシンシャ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>datetime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>delete_flag</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>削除フラグ</t>
-    <rPh sb="0" eb="2">
-      <t>サクジョ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>boolean</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>default=false</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>mysql+flyway</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お祝い</t>
-    <rPh sb="1" eb="2">
-      <t>イワ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>celerbration_reply</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お祝い書き込み</t>
-    <rPh sb="1" eb="2">
-      <t>イワ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>コ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>celerbration_no</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>celerbrationテーブルのFK</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>String(500)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・header</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -401,17 +130,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>String array</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>IDを記録</t>
-    <rPh sb="3" eb="5">
-      <t>キロク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・お祝い+お祝い書き込みのneed_readの数を表示</t>
     <rPh sb="2" eb="3">
       <t>イワ</t>
@@ -493,45 +211,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PK</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>type</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ユーザタイプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ネーム</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>password</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>パスワード</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>profile_image_url</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>プロフィール写真のURL</t>
-    <rPh sb="6" eb="8">
-      <t>シャシン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・以前ページボタンを押下</t>
     <rPh sb="1" eb="3">
       <t>イゼン</t>
@@ -658,16 +337,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>・作成・修正ページ</t>
-    <rPh sb="1" eb="3">
-      <t>サクセイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シュウセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>・Junit</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -706,96 +375,51 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>read_count</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>読んだ数</t>
-    <rPh sb="0" eb="1">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>スウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>profile_image</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>プロフィール管理テーブル</t>
+    <t>結婚のお祝いを記録しておきたい。できれば、書き込みと通知ができてやり取りができればと思います。</t>
+    <rPh sb="0" eb="2">
+      <t>ケッコン</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>イワ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>キロク</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ツウチ</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>ト</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>オモ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>お祝いリスト表示APIを利用し、リストを表示する。</t>
+    <rPh sb="1" eb="2">
+      <t>イワ</t>
+    </rPh>
     <rPh sb="6" eb="8">
-      <t>カンリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>profile_image_no</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>プロフィール管理テーブルFK</t>
-    <rPh sb="6" eb="8">
-      <t>カンリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FK</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1:管理者
-2:非ユーザ
-3:KAKAOユーザ
-4:Lineユーザ</t>
-    <rPh sb="2" eb="5">
-      <t>カンリシャ</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>ヒ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>userテーブルのFK</t>
-  </si>
-  <si>
-    <t>ユーザ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>unread_user</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>まだ確認していない人</t>
-    <rPh sb="2" eb="4">
-      <t>カクニン</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ヒト</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お祝い番号</t>
-    <rPh sb="3" eb="5">
-      <t>バンゴウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ユーザID</t>
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>frontend</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3591,18 +3215,6 @@
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>* </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>一回登録すると変更ができません。</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-        </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
@@ -4442,185 +4054,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>0</v>
+      <c r="B7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B11" t="s">
-        <v>53</v>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B12" t="s">
-        <v>54</v>
+      <c r="A12" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" t="s">
-        <v>99</v>
+      <c r="B13" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B20" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C31" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="C32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="B33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C34" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.4">
-      <c r="C36" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -4631,42 +4184,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97BE568E-ACF5-42CE-B1A7-90711DB6A05D}">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97434556-6B23-4BF1-9CB6-03B00EDF4972}">
+  <dimension ref="A36:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97434556-6B23-4BF1-9CB6-03B00EDF4972}">
-  <dimension ref="A1:D53"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4677,618 +4199,17 @@
     <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C13" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>114</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>112</v>
-      </c>
-      <c r="B27" t="s">
-        <v>113</v>
-      </c>
-      <c r="C27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" t="s">
-        <v>115</v>
-      </c>
-      <c r="C33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A36" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>109</v>
-      </c>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A37" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" t="s">
-        <v>38</v>
-      </c>
-      <c r="D40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" t="s">
-        <v>21</v>
-      </c>
-      <c r="D41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C46" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" t="s">
-        <v>18</v>
-      </c>
-      <c r="C47" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>30</v>
-      </c>
-      <c r="B49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B50" t="s">
-        <v>35</v>
-      </c>
-      <c r="C50" t="s">
-        <v>21</v>
-      </c>
-      <c r="D50" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>32</v>
-      </c>
-      <c r="B51" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" t="s">
-        <v>38</v>
-      </c>
-      <c r="D51" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>34</v>
-      </c>
-      <c r="B52" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" t="s">
-        <v>21</v>
-      </c>
-      <c r="D52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>39</v>
-      </c>
-      <c r="B53" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" t="s">
-        <v>41</v>
-      </c>
-      <c r="D53" t="s">
-        <v>42</v>
-      </c>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -5296,12 +4217,29 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD494820-4783-46C6-9638-7271400D1637}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFAD6C30-5A6A-4F1A-A99D-6F71EF6C1A28}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5311,37 +4249,37 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D10" s="2" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -5352,17 +4290,17 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D13" s="2" t="s">
-        <v>64</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C14" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.4">
@@ -5370,7 +4308,7 @@
     </row>
     <row r="18" spans="4:4" x14ac:dyDescent="0.4">
       <c r="D18" s="2" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5385,7 +4323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB63D199-DE6C-43DE-9E1E-C8D76622D48E}">
   <dimension ref="K34:M48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -5393,72 +4331,72 @@
   <sheetData>
     <row r="34" spans="11:13" x14ac:dyDescent="0.4">
       <c r="K34" t="s">
-        <v>79</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L35" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M36" s="2" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L37" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M38" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L39" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
     </row>
     <row r="40" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M40" t="s">
-        <v>83</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="11:13" x14ac:dyDescent="0.4">
       <c r="K42" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L43" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M44" s="2" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L45" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M46" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="11:13" x14ac:dyDescent="0.4">
       <c r="L47" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="11:13" x14ac:dyDescent="0.4">
       <c r="M48" s="2" t="s">
-        <v>90</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -5473,14 +4411,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -5488,4 +4426,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231B9156-F317-446E-BBB1-DB7B32D9520C}">
+  <dimension ref="B2:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623344E4-E6C4-43A8-967A-19180C0BF382}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add design to celebration list,write,delete,modify
</commit_message>
<xml_diff>
--- a/document/基本設計書/お祝い.xlsx
+++ b/document/基本設計書/お祝い.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\azusato\document\基本設計書\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\azusato\document\基本設計書\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AE594A-9D4E-4067-A696-2A0CEE4223FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F784EB-B3BF-4B01-8E59-0AE5755E711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="2400" windowWidth="21600" windowHeight="11385" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9885" yWindow="1035" windowWidth="14100" windowHeight="13830" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,6 @@
     <sheet name="header(html)" sheetId="6" r:id="rId4"/>
     <sheet name="リストページ(html)" sheetId="4" r:id="rId5"/>
     <sheet name="作成・修正ページ(html)" sheetId="7" r:id="rId6"/>
-    <sheet name="リストページ" sheetId="10" r:id="rId7"/>
-    <sheet name="Sheet4" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>ページ</t>
     <phoneticPr fontId="1"/>
@@ -400,26 +398,6 @@
     <rPh sb="42" eb="43">
       <t>オモ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>お祝いリスト表示APIを利用し、リストを表示する。</t>
-    <rPh sb="1" eb="2">
-      <t>イワ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="12" eb="14">
-      <t>リヨウ</t>
-    </rPh>
-    <rPh sb="20" eb="22">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>frontend</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -490,7 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4238,7 +4216,7 @@
   </sheetPr>
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -4323,7 +4301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB63D199-DE6C-43DE-9E1E-C8D76622D48E}">
   <dimension ref="K34:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -4410,8 +4388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD9DB05-932A-4FAA-A0C5-773A5804E9B9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -4426,48 +4404,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231B9156-F317-446E-BBB1-DB7B32D9520C}">
-  <dimension ref="B2:B5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623344E4-E6C4-43A8-967A-19180C0BF382}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>